<commit_message>
CPU: Moorsches Gesetz überarbeitet.
</commit_message>
<xml_diff>
--- a/1-basics/3-cpu/assets/moores-law.xlsx
+++ b/1-basics/3-cpu/assets/moores-law.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Repos/teach/computer/1-basics/3-cpu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Repos/teach/computer/1-basics/3-cpu/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B46573-D3D2-B741-88CA-C58B3523BED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688FE1D9-4DCD-D243-9F73-7AFDDA9AA511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" xr2:uid="{C683C1FC-DE17-534E-B354-21DF64DC3FF2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{C683C1FC-DE17-534E-B354-21DF64DC3FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Jahr</t>
   </si>
   <si>
-    <t>Intel Desktop</t>
-  </si>
-  <si>
     <t>Apple</t>
   </si>
   <si>
@@ -156,6 +153,18 @@
   </si>
   <si>
     <t>AMD Ryzen 9</t>
+  </si>
+  <si>
+    <t>AMD Name</t>
+  </si>
+  <si>
+    <t>Apple Name</t>
+  </si>
+  <si>
+    <t>Intel Name</t>
+  </si>
+  <si>
+    <t>Intel</t>
   </si>
 </sst>
 </file>
@@ -164,7 +173,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -214,14 +223,109 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -249,6 +353,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Anzahl</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> Transistoren in Desktop-Prozessoren</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -285,327 +419,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> Intel Desktop </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="15"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-5BFD-524B-9784-87204E77E029}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$1:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>Jahr</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1971</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1972</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1973</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1974</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1975</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1976</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1977</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1978</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1979</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1980</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1981</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1982</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1983</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1984</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1985</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1986</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1987</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1988</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1989</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1990</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1991</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1992</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1993</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1994</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1995</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1996</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$E$1:$E$51</c:f>
-              <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2250</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>134000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>275000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1180235</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3100000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5500000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7500000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9500000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>42000000</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>112000000</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>228000000</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>362000000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>411000000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>731000000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1170000000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1400000000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2600000000</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3200000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5BFD-524B-9784-87204E77E029}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$G$1</c:f>
@@ -619,9 +434,7 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -642,197 +455,192 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$1:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="51"/>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>Jahr</c:v>
+                  <c:v>1971</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1972</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1973</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1974</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1975</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1976</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1977</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1978</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1979</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1980</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>1981</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>1982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>1983</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>1984</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>1985</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>1986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>1987</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>1988</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>1989</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1998</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1999</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2000</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2001</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2002</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2003</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2004</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2005</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2006</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2007</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2008</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2009</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2010</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2011</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2012</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2013</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2014</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2015</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2016</c:v>
+                  <c:v>2017</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2017</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2018</c:v>
+                  <c:v>2019</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="50">
                   <c:v>2020</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$1:$G$51</c:f>
+              <c:f>Tabelle1!$G$2:$G$51</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="50"/>
+                <c:pt idx="42">
+                  <c:v>1000000000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1000000000</c:v>
+                  <c:v>2000000000</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>2000000000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2000000000</c:v>
+                  <c:v>3300000000</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3300000000</c:v>
+                  <c:v>4300000000</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4300000000</c:v>
+                  <c:v>6900000000</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6900000000</c:v>
+                  <c:v>9500000000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9500000000</c:v>
-                </c:pt>
-                <c:pt idx="50">
                   <c:v>11800000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -842,6 +650,328 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-5BFD-524B-9784-87204E77E029}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Intel </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2BC1-F948-A2BE-2250998E14BA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$2:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>134000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>275000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1180235</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3100000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5500000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9500000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42000000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>112000000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>228000000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>362000000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>411000000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>731000000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1170000000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1400000000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2600000000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3200000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5BFD-524B-9784-87204E77E029}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -861,9 +991,7 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -873,9 +1001,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -892,9 +1018,7 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
@@ -907,11 +1031,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
+                <a:noFill/>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
@@ -922,11 +1042,170 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$C$2:$C$51</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0_-;\-* #\,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="25">
                   <c:v>4300000</c:v>
@@ -1000,7 +1279,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1031,12 +1310,13 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -1048,6 +1328,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Anzahl</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> Transistoren</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1123,7 +1463,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1714,15 +2054,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>451069</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>189771</xdr:rowOff>
+      <xdr:colOff>203968</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>102409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>519678</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>71822</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>69275</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14522</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1748,6 +2088,22 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B2660481-D93C-CB4D-AFDA-6E7B6F88B250}" name="Tabelle1" displayName="Tabelle1" ref="A1:G51" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowCellStyle="Komma" dataCellStyle="Komma">
+  <autoFilter ref="A1:G51" xr:uid="{E5104F93-17F1-1E4F-832C-87475B38B4B2}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{DE0539AD-060C-A040-80FD-DA53EF303462}" name="Jahr"/>
+    <tableColumn id="2" xr3:uid="{2CFE8D6B-376F-DA49-9263-5F41EE721715}" name="AMD Name"/>
+    <tableColumn id="3" xr3:uid="{D58A3D28-766C-9245-90C0-4E00709E3C06}" name="AMD" dataDxfId="2" dataCellStyle="Komma"/>
+    <tableColumn id="4" xr3:uid="{723B76AF-9296-BD47-A1FB-DBDCE5B94C0A}" name="Intel Name"/>
+    <tableColumn id="5" xr3:uid="{8982BF59-05BD-A341-A368-6C4AE8CD6661}" name="Intel" dataDxfId="1" dataCellStyle="Komma"/>
+    <tableColumn id="6" xr3:uid="{B9B119BD-CA8F-364D-A614-68A2986F2671}" name="Apple Name"/>
+    <tableColumn id="7" xr3:uid="{8868E7B2-6221-8C4D-A146-9B4BECB30B3B}" name="Apple" dataDxfId="0" dataCellStyle="Komma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2049,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA312EA-8934-7241-9EA2-DE2F96CBB252}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2058,7 +2414,8 @@
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2067,22 +2424,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2090,7 +2447,7 @@
         <v>1971</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3">
         <v>2250</v>
@@ -2101,7 +2458,7 @@
         <v>1972</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3">
         <v>3500</v>
@@ -2117,7 +2474,7 @@
         <v>1974</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>6000</v>
@@ -2133,7 +2490,7 @@
         <v>1976</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3">
         <v>6500</v>
@@ -2149,7 +2506,7 @@
         <v>1978</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="3">
         <v>29000</v>
@@ -2175,7 +2532,7 @@
         <v>1982</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3">
         <v>134000</v>
@@ -2196,7 +2553,7 @@
         <v>1985</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3">
         <v>275000</v>
@@ -2222,7 +2579,7 @@
         <v>1989</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3">
         <v>1180235</v>
@@ -2248,7 +2605,7 @@
         <v>1993</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="3">
         <v>3100000</v>
@@ -2264,7 +2621,7 @@
         <v>1995</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" s="3">
         <v>5500000</v>
@@ -2275,7 +2632,7 @@
         <v>1996</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3">
         <v>4300000</v>
@@ -2286,13 +2643,13 @@
         <v>1997</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3">
         <v>8800000</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="3">
         <v>7500000</v>
@@ -2308,13 +2665,13 @@
         <v>1999</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3">
         <v>22000000</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" s="3">
         <v>9500000</v>
@@ -2325,7 +2682,7 @@
         <v>2000</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" s="3">
         <v>42000000</v>
@@ -2346,7 +2703,7 @@
         <v>2003</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="3">
         <v>105900000</v>
@@ -2357,7 +2714,7 @@
         <v>2004</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" s="3">
         <v>112000000</v>
@@ -2368,7 +2725,7 @@
         <v>2005</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="3">
         <v>228000000</v>
@@ -2379,7 +2736,7 @@
         <v>2006</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E37" s="3">
         <v>362000000</v>
@@ -2390,13 +2747,13 @@
         <v>2007</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="3">
         <v>463000000</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E38" s="3">
         <v>411000000</v>
@@ -2407,7 +2764,7 @@
         <v>2008</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E39" s="3">
         <v>731000000</v>
@@ -2423,7 +2780,7 @@
         <v>2010</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E41" s="3">
         <v>1170000000</v>
@@ -2439,13 +2796,13 @@
         <v>2012</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="3">
         <v>1200000000</v>
       </c>
       <c r="D43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E43" s="3">
         <v>1400000000</v>
@@ -2456,7 +2813,7 @@
         <v>2013</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" s="3">
         <v>1000000000</v>
@@ -2467,13 +2824,13 @@
         <v>2014</v>
       </c>
       <c r="D45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E45" s="3">
         <v>2600000000</v>
       </c>
       <c r="F45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45" s="3">
         <v>2000000000</v>
@@ -2484,7 +2841,7 @@
         <v>2015</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G46" s="3">
         <v>2000000000</v>
@@ -2495,13 +2852,13 @@
         <v>2016</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E47" s="3">
         <v>3200000000</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G47" s="3">
         <v>3300000000</v>
@@ -2512,13 +2869,13 @@
         <v>2017</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C48" s="3">
         <v>4800000000</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G48" s="3">
         <v>4300000000</v>
@@ -2529,7 +2886,7 @@
         <v>2018</v>
       </c>
       <c r="F49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G49" s="3">
         <v>6900000000</v>
@@ -2540,13 +2897,13 @@
         <v>2019</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" s="3">
         <v>9890000000</v>
       </c>
       <c r="F50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G50" s="3">
         <v>9500000000</v>
@@ -2557,7 +2914,7 @@
         <v>2020</v>
       </c>
       <c r="F51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G51" s="3">
         <v>11800000000</v>
@@ -2566,5 +2923,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>